<commit_message>
Updates since last meeting (8/7)
</commit_message>
<xml_diff>
--- a/KeyValueDatabases.xlsx
+++ b/KeyValueDatabases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anthonys_Documents\Uni_Stuttgart\Forschungsprojekt\Key-Value-Datenspeichern-FP-2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF83798B-F652-4977-A015-DB98AB769290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88EBD7BA-CFEF-4BD8-878E-7506245F9029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5280" windowWidth="29040" windowHeight="15840" xr2:uid="{92F50C3F-08B8-4F3D-A3AD-7E997F6070BE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{92F50C3F-08B8-4F3D-A3AD-7E997F6070BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="154">
   <si>
     <t>Vergleich von Key-Value Datenspeichern</t>
   </si>
@@ -516,9 +516,6 @@
     <t>möglich - Auto-Clustering, Daten werden automatisch über mehrere Redis-knoten geteilt. Datensätze werden automatische über mehrere Knoten gesplittet. Operationen können weitergeführt werden, auch wenn eine Teilmenge von Knoten fehlschlagen.</t>
   </si>
   <si>
-    <t>make diagram for Test-verlauf</t>
-  </si>
-  <si>
     <t>To-do:</t>
   </si>
   <si>
@@ -528,13 +525,38 @@
     <t>write in Java</t>
   </si>
   <si>
-    <t>generate data on the go, not store raw data? - create data</t>
-  </si>
-  <si>
     <t xml:space="preserve">decide what criteria to test </t>
   </si>
   <si>
-    <t>binary tree: nodes are hashed values, fixed 4-16KB of data</t>
+    <t>https://github.com/brianfrankcooper/YCSB</t>
+  </si>
+  <si>
+    <t>Reference performance comparison</t>
+  </si>
+  <si>
+    <t>Properties Tested:</t>
+  </si>
+  <si>
+    <t>https://www.guru99.com/data-testing.html</t>
+  </si>
+  <si>
+    <t>binary tree: nodes are hashed values, fixed 4KB of data</t>
+  </si>
+  <si>
+    <t>one more library DB (like MapDB)</t>
+  </si>
+  <si>
+    <t>generate b-tree and store values directly into DB -- no need for random values</t>
+  </si>
+  <si>
+    <t>look for papers, similar to what we are doing</t>
+  </si>
+  <si>
+    <t>Datenbank Tabellen Testing -  Daten Validierung (Key gültig? Value richtig? Tabelle/Cluster erstellt?)
+Trigger Testing - Benötigte Zeit, Anzahl Operationen pro Sekunde (Schreiben, Löschen, Lesen/Queries -- INSERT, UPDATE(?), GET, DELETE)</t>
+  </si>
+  <si>
+    <t>See how we can use YCSB for our purpose</t>
   </si>
 </sst>
 </file>
@@ -611,7 +633,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -633,6 +655,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -664,7 +689,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>752475</xdr:colOff>
+      <xdr:colOff>1681</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>991720</xdr:rowOff>
     </xdr:to>
@@ -1016,10 +1041,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53819EDE-CF27-4B86-AEAB-051F92A3B4AB}">
-  <dimension ref="A1:P22"/>
+  <dimension ref="A1:Z22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1032,14 +1057,19 @@
     <col min="8" max="9" width="23" customWidth="1"/>
     <col min="10" max="10" width="22.7109375" customWidth="1"/>
     <col min="11" max="11" width="22.85546875" customWidth="1"/>
+    <col min="16" max="16" width="22.7109375" customWidth="1"/>
+    <col min="23" max="23" width="34.42578125" customWidth="1"/>
+    <col min="24" max="24" width="22.7109375" customWidth="1"/>
+    <col min="25" max="25" width="57" customWidth="1"/>
+    <col min="26" max="26" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1073,8 +1103,11 @@
       <c r="M3" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>129</v>
       </c>
@@ -1105,8 +1138,20 @@
       <c r="J4" s="5" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" ht="144" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W4" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="X4" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="144" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
@@ -1141,7 +1186,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>16</v>
       </c>
@@ -1171,7 +1216,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>130</v>
       </c>
@@ -1201,19 +1246,19 @@
         <v>111</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="N7" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="O7" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="O7" s="5" t="s">
-        <v>143</v>
-      </c>
       <c r="P7" s="5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="183.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="183.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>23</v>
       </c>
@@ -1245,16 +1290,22 @@
         <v>81</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="O8" s="5" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="255" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="P8" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q8" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="255" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>115</v>
       </c>
@@ -1285,8 +1336,10 @@
       <c r="J9" s="5" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M9" s="2"/>
+      <c r="N9" s="9"/>
+    </row>
+    <row r="10" spans="1:26" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>118</v>
       </c>
@@ -1318,7 +1371,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
@@ -1348,7 +1401,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>39</v>
       </c>
@@ -1380,7 +1433,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>43</v>
       </c>
@@ -1412,7 +1465,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="360" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" ht="360" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>48</v>
       </c>
@@ -1445,7 +1498,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>52</v>
       </c>
@@ -1477,7 +1530,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>58</v>
       </c>
@@ -1623,9 +1676,10 @@
     <hyperlink ref="F12" r:id="rId24" xr:uid="{C6B2DCFA-F793-40CB-8A11-0B6C09B10D08}"/>
     <hyperlink ref="F13" r:id="rId25" xr:uid="{BBEEB0EE-E2E3-459F-9E79-0FB80E4EBE96}"/>
     <hyperlink ref="J15" r:id="rId26" display="https://www.quora.com/How-scalable-is-Redis                                            Partitioning:_x000a_Since the data is in key-value format, its easy to distribute them into different partitions. In this way, we don't have to rely on a single computer. Same time, the overall capacity of Redis instance is equal to the number of machines in the cluster (i.e., it can make use of complete resources in your cluster)._x000a_Replication:_x000a_Redis follows master-slave replication, that means you can have one master and many slaves (and each slave can have slaves - like a graph). It allows distributing the load across machines and making use of memory of all the machines in the cluster (also shared bandwidth)._x000a_Failover:_x000a_Redis Sentinal helps to manage Redis instances. If a master goes down, Sentinal automatically starts a process that can promote Slave node into Master._x000a_Also, it updates the clients to use new master instead of the old._x000a_Note: Redis configurations are eventually-consistent._x000a_Connections:_x000a_Redis uses multiplexing and non-blocking I/O techniques to handle incoming connections. It just increases the availability of the Redis instance._x000a_Recovery:_x000a_One of the major problem with large scale is, How to recover incase of failover. Redis Persistence can address this. The RDB persistence performs point-in-time snapshots of your dataset at specified intervals. These snapshots are completely configurable and can be transferred to different datacenter for recovery purposes." xr:uid="{AE6EB149-477D-4377-A473-0485F04F51F9}"/>
+    <hyperlink ref="X4" r:id="rId27" xr:uid="{9BF6AB1B-E662-4576-905A-0F30A8D261CC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId27"/>
-  <drawing r:id="rId28"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId28"/>
+  <drawing r:id="rId29"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updates since last meeting (21/7)
</commit_message>
<xml_diff>
--- a/KeyValueDatabases.xlsx
+++ b/KeyValueDatabases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anthonys_Documents\Uni_Stuttgart\Forschungsprojekt\Key-Value-Datenspeichern-FP-2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88EBD7BA-CFEF-4BD8-878E-7506245F9029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE02A71-4515-41D0-A839-2A65BAF2B4FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{92F50C3F-08B8-4F3D-A3AD-7E997F6070BE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="156">
   <si>
     <t>Vergleich von Key-Value Datenspeichern</t>
   </si>
@@ -557,6 +557,19 @@
   </si>
   <si>
     <t>See how we can use YCSB for our purpose</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>1. Datenbank starten
+2. Daten erzeugen
+3. Daten ins Datenbank schreiben/streamen (Test INSERT)
+(3.5. Data validation)
+4. Test GET
+5. Test UPDATE
+(5.5 Test DELETE)
+6. Datenbank herunterfahren</t>
   </si>
 </sst>
 </file>
@@ -1043,8 +1056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53819EDE-CF27-4B86-AEAB-051F92A3B4AB}">
   <dimension ref="A1:Z22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView tabSelected="1" topLeftCell="F4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y5" sqref="Y5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1185,6 +1198,9 @@
       <c r="K5" s="2" t="s">
         <v>85</v>
       </c>
+      <c r="Y5" s="2" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="6" spans="1:26" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -1303,6 +1319,9 @@
       </c>
       <c r="Q8" s="5" t="s">
         <v>153</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="255" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added Zwischenvortrag ppt, update since last meeting (31/7)
</commit_message>
<xml_diff>
--- a/KeyValueDatabases.xlsx
+++ b/KeyValueDatabases.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anthonys_Documents\Uni_Stuttgart\Forschungsprojekt\Key-Value-Datenspeichern-FP-2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE02A71-4515-41D0-A839-2A65BAF2B4FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5CEEE61-9754-4DE3-A5BD-7634C83DF618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{92F50C3F-08B8-4F3D-A3AD-7E997F6070BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="157">
   <si>
     <t>Vergleich von Key-Value Datenspeichern</t>
   </si>
@@ -525,9 +526,6 @@
     <t>write in Java</t>
   </si>
   <si>
-    <t xml:space="preserve">decide what criteria to test </t>
-  </si>
-  <si>
     <t>https://github.com/brianfrankcooper/YCSB</t>
   </si>
   <si>
@@ -543,13 +541,7 @@
     <t>binary tree: nodes are hashed values, fixed 4KB of data</t>
   </si>
   <si>
-    <t>one more library DB (like MapDB)</t>
-  </si>
-  <si>
     <t>generate b-tree and store values directly into DB -- no need for random values</t>
-  </si>
-  <si>
-    <t>look for papers, similar to what we are doing</t>
   </si>
   <si>
     <t>Datenbank Tabellen Testing -  Daten Validierung (Key gültig? Value richtig? Tabelle/Cluster erstellt?)
@@ -557,9 +549,6 @@
   </si>
   <si>
     <t>See how we can use YCSB for our purpose</t>
-  </si>
-  <si>
-    <t>+</t>
   </si>
   <si>
     <t>1. Datenbank starten
@@ -570,6 +559,22 @@
 5. Test UPDATE
 (5.5 Test DELETE)
 6. Datenbank herunterfahren</t>
+  </si>
+  <si>
+    <t>Zwischen-presentation</t>
+  </si>
+  <si>
+    <t>Look at papers, find what we can use (formats, sources, results)</t>
+  </si>
+  <si>
+    <t>Figure out how to solve our problems/how to find answers</t>
+  </si>
+  <si>
+    <t>1. Benchmarks vergleichen
+2. Papers vergleichen</t>
+  </si>
+  <si>
+    <t>H2Database - MVStore</t>
   </si>
 </sst>
 </file>
@@ -654,7 +659,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -672,6 +676,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1054,10 +1061,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53819EDE-CF27-4B86-AEAB-051F92A3B4AB}">
-  <dimension ref="A1:Z22"/>
+  <dimension ref="A1:Z21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Y5" sqref="Y5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1117,400 +1124,404 @@
         <v>86</v>
       </c>
       <c r="Y3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="X4" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="Z4" s="2" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="W4" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="X4" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="Y4" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="Z4" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
     <row r="5" spans="1:26" ht="144" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="4" t="s">
         <v>107</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>85</v>
       </c>
       <c r="Y5" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="183.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q8" s="4"/>
+    </row>
+    <row r="9" spans="1:26" ht="255" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="M9" s="2"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="P9" s="2" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="6" spans="1:26" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="5" t="s">
+      <c r="Q9" s="9" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="360" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="M7" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="N7" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="O7" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="P7" s="5" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="183.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="M8" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="N8" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="O8" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="P8" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="Q8" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="255" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="M9" s="2"/>
-      <c r="N9" s="9"/>
-    </row>
-    <row r="10" spans="1:26" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="360" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5" t="s">
+      <c r="F14" s="4"/>
+      <c r="G14" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="H14" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="I14" s="5" t="s">
+      <c r="I14" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="J14" s="5" t="s">
+      <c r="J14" s="4" t="s">
         <v>98</v>
       </c>
       <c r="K14" s="2" t="s">
@@ -1518,154 +1529,151 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="G15" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="H15" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="I15" s="5" t="s">
+      <c r="I15" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="J15" s="6" t="s">
+      <c r="J15" s="5" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
     </row>
     <row r="17" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
     </row>
     <row r="18" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
     </row>
     <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5" t="s">
+      <c r="F19" s="4"/>
+      <c r="G19" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
     </row>
     <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="F20" s="5"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
     </row>
     <row r="21" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G21" s="4"/>
-    </row>
-    <row r="22" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G22" s="3"/>
+      <c r="G21" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1701,4 +1709,468 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId28"/>
   <drawing r:id="rId29"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BFE27C2-1312-4A04-AF7F-1C5ECB1703A1}">
+  <dimension ref="A1:H18"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="27" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="31.140625" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" customWidth="1"/>
+    <col min="7" max="7" width="36.42578125" customWidth="1"/>
+    <col min="8" max="8" width="27.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="157.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="141" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="204" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="141" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="229.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F18" s="4"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="4"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E17" r:id="rId1" display="https://dbmx.net/tkrzw/" xr:uid="{DF73007F-F515-4520-ABD1-E0FE616DA734}"/>
+    <hyperlink ref="E18" r:id="rId2" display="https://github.com/hazelcast/hazelcast" xr:uid="{C759E358-5FA7-406D-B1A4-2D7EE8085E42}"/>
+    <hyperlink ref="H13" r:id="rId3" display="https://www.quora.com/How-scalable-is-Redis                                            Partitioning:_x000a_Since the data is in key-value format, its easy to distribute them into different partitions. In this way, we don't have to rely on a single computer. Same time, the overall capacity of Redis instance is equal to the number of machines in the cluster (i.e., it can make use of complete resources in your cluster)._x000a_Replication:_x000a_Redis follows master-slave replication, that means you can have one master and many slaves (and each slave can have slaves - like a graph). It allows distributing the load across machines and making use of memory of all the machines in the cluster (also shared bandwidth)._x000a_Failover:_x000a_Redis Sentinal helps to manage Redis instances. If a master goes down, Sentinal automatically starts a process that can promote Slave node into Master._x000a_Also, it updates the clients to use new master instead of the old._x000a_Note: Redis configurations are eventually-consistent._x000a_Connections:_x000a_Redis uses multiplexing and non-blocking I/O techniques to handle incoming connections. It just increases the availability of the Redis instance._x000a_Recovery:_x000a_One of the major problem with large scale is, How to recover incase of failover. Redis Persistence can address this. The RDB persistence performs point-in-time snapshots of your dataset at specified intervals. These snapshots are completely configurable and can be transferred to different datacenter for recovery purposes." xr:uid="{25CC01B7-3574-489A-818D-70D793877ADC}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added comments on ppt draft, revisioned ppt
</commit_message>
<xml_diff>
--- a/KeyValueDatabases.xlsx
+++ b/KeyValueDatabases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anthonys_Documents\Uni_Stuttgart\Forschungsprojekt\Key-Value-Datenspeichern-FP-2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5CEEE61-9754-4DE3-A5BD-7634C83DF618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BBD2C55-8E9E-4232-9EC2-8A2B34A06A8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{92F50C3F-08B8-4F3D-A3AD-7E997F6070BE}"/>
+    <workbookView xWindow="1245" yWindow="8190" windowWidth="37155" windowHeight="12810" activeTab="1" xr2:uid="{92F50C3F-08B8-4F3D-A3AD-7E997F6070BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="173">
   <si>
     <t>Vergleich von Key-Value Datenspeichern</t>
   </si>
@@ -575,6 +575,57 @@
   </si>
   <si>
     <t>H2Database - MVStore</t>
+  </si>
+  <si>
+    <t>WhiteDB</t>
+  </si>
+  <si>
+    <t>C API</t>
+  </si>
+  <si>
+    <t>Persistent (von RAM auf Festplatte)</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>http://whitedb.org/</t>
+  </si>
+  <si>
+    <t>http://whitedb.org/tutorial.html</t>
+  </si>
+  <si>
+    <t>http://whitedb.org/install.html</t>
+  </si>
+  <si>
+    <t>Hängt von Größe der RAM ab</t>
+  </si>
+  <si>
+    <t>Nicht möglich, nur 1 Instanz in shared memory/RAM ist</t>
+  </si>
+  <si>
+    <t>MVStore</t>
+  </si>
+  <si>
+    <t>Map (Java)</t>
+  </si>
+  <si>
+    <t>https://www.h2database.com/html/mvstore.html</t>
+  </si>
+  <si>
+    <t>möglich: braucht aber zusätzliche Computer</t>
+  </si>
+  <si>
+    <t>mit neue Cluster?</t>
+  </si>
+  <si>
+    <t>"For fully scalable concurrent write operations to a map (in-memory and to disk),
+the map could be split into multiple maps in different stores ('sharding').
+The plan is to add such a mechanism later when needed."</t>
+  </si>
+  <si>
+    <t>https://github.com/h2database/h2database/blob/master/h2/src/docsrc/html/mvstore.html
+315-317</t>
   </si>
 </sst>
 </file>
@@ -651,16 +702,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1061,10 +1109,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53819EDE-CF27-4B86-AEAB-051F92A3B4AB}">
-  <dimension ref="A1:Z21"/>
+  <dimension ref="A1:Z22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G22" sqref="G21:K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1128,40 +1176,40 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="3" t="s">
         <v>87</v>
       </c>
       <c r="W4" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="X4" s="8" t="s">
+      <c r="X4" s="7" t="s">
         <v>143</v>
       </c>
       <c r="Y4" s="2" t="s">
@@ -1172,34 +1220,34 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="144" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="3" t="s">
         <v>107</v>
       </c>
       <c r="K5" s="2" t="s">
@@ -1210,318 +1258,318 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4" t="s">
+      <c r="F6" s="3"/>
+      <c r="G6" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="J6" s="3" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4" t="s">
+      <c r="F7" s="3"/>
+      <c r="G7" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I7" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J7" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="M7" s="4" t="s">
+      <c r="M7" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="N7" s="4" t="s">
+      <c r="N7" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="O7" s="4" t="s">
+      <c r="O7" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="P7" s="4" t="s">
+      <c r="P7" s="3" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="183.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="M8" s="4" t="s">
+      <c r="M8" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="N8" s="4" t="s">
+      <c r="N8" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="O8" s="4" t="s">
+      <c r="O8" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="P8" s="4" t="s">
+      <c r="P8" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="Q8" s="4"/>
+      <c r="Q8" s="3"/>
     </row>
     <row r="9" spans="1:26" ht="255" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I9" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="J9" s="3" t="s">
         <v>90</v>
       </c>
       <c r="M9" s="2"/>
-      <c r="N9" s="8"/>
+      <c r="N9" s="7"/>
       <c r="O9" s="2" t="s">
         <v>152</v>
       </c>
       <c r="P9" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="Q9" s="9" t="s">
+      <c r="Q9" s="8" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I10" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="J10" s="3" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4" t="s">
+      <c r="F11" s="3"/>
+      <c r="G11" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="J11" s="3" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H12" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="I12" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="J12" s="4" t="s">
+      <c r="J12" s="3" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G13" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H13" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="I13" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="J13" s="4" t="s">
+      <c r="J13" s="3" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="360" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4" t="s">
+      <c r="F14" s="3"/>
+      <c r="G14" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="I14" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="J14" s="3" t="s">
         <v>98</v>
       </c>
       <c r="K14" s="2" t="s">
@@ -1529,151 +1577,211 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="G15" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="H15" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="I15" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="J15" s="5" t="s">
+      <c r="J15" s="4" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-    </row>
-    <row r="17" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+    </row>
+    <row r="17" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-    </row>
-    <row r="18" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+    </row>
+    <row r="18" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-    </row>
-    <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+    </row>
+    <row r="19" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4" t="s">
+      <c r="F19" s="3"/>
+      <c r="G19" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-    </row>
-    <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+    </row>
+    <row r="20" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F20" s="4"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-    </row>
-    <row r="21" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G21" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+    </row>
+    <row r="21" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="165" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="F22" s="3"/>
+      <c r="G22" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="K22" s="7" t="s">
+        <v>172</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1704,19 +1812,20 @@
     <hyperlink ref="F13" r:id="rId25" xr:uid="{BBEEB0EE-E2E3-459F-9E79-0FB80E4EBE96}"/>
     <hyperlink ref="J15" r:id="rId26" display="https://www.quora.com/How-scalable-is-Redis                                            Partitioning:_x000a_Since the data is in key-value format, its easy to distribute them into different partitions. In this way, we don't have to rely on a single computer. Same time, the overall capacity of Redis instance is equal to the number of machines in the cluster (i.e., it can make use of complete resources in your cluster)._x000a_Replication:_x000a_Redis follows master-slave replication, that means you can have one master and many slaves (and each slave can have slaves - like a graph). It allows distributing the load across machines and making use of memory of all the machines in the cluster (also shared bandwidth)._x000a_Failover:_x000a_Redis Sentinal helps to manage Redis instances. If a master goes down, Sentinal automatically starts a process that can promote Slave node into Master._x000a_Also, it updates the clients to use new master instead of the old._x000a_Note: Redis configurations are eventually-consistent._x000a_Connections:_x000a_Redis uses multiplexing and non-blocking I/O techniques to handle incoming connections. It just increases the availability of the Redis instance._x000a_Recovery:_x000a_One of the major problem with large scale is, How to recover incase of failover. Redis Persistence can address this. The RDB persistence performs point-in-time snapshots of your dataset at specified intervals. These snapshots are completely configurable and can be transferred to different datacenter for recovery purposes." xr:uid="{AE6EB149-477D-4377-A473-0485F04F51F9}"/>
     <hyperlink ref="X4" r:id="rId27" xr:uid="{9BF6AB1B-E662-4576-905A-0F30A8D261CC}"/>
+    <hyperlink ref="K22" r:id="rId28" xr:uid="{DEF160FC-0BF2-45C7-90A1-913E51ACA468}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId28"/>
-  <drawing r:id="rId29"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId29"/>
+  <drawing r:id="rId30"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BFE27C2-1312-4A04-AF7F-1C5ECB1703A1}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17:I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1758,418 +1867,428 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="157.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="141" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="3" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="3" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="3" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="204" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="3" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="3" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="3" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="141" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="3" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="3" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="229.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H12" s="3" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G13" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="H13" s="4" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
     </row>
     <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-    </row>
-    <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="4" t="s">
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="H17" s="4"/>
-    </row>
-    <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E18" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="F18" s="4"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="4"/>
+      <c r="E18" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>172</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E17" r:id="rId1" display="https://dbmx.net/tkrzw/" xr:uid="{DF73007F-F515-4520-ABD1-E0FE616DA734}"/>
-    <hyperlink ref="E18" r:id="rId2" display="https://github.com/hazelcast/hazelcast" xr:uid="{C759E358-5FA7-406D-B1A4-2D7EE8085E42}"/>
-    <hyperlink ref="H13" r:id="rId3" display="https://www.quora.com/How-scalable-is-Redis                                            Partitioning:_x000a_Since the data is in key-value format, its easy to distribute them into different partitions. In this way, we don't have to rely on a single computer. Same time, the overall capacity of Redis instance is equal to the number of machines in the cluster (i.e., it can make use of complete resources in your cluster)._x000a_Replication:_x000a_Redis follows master-slave replication, that means you can have one master and many slaves (and each slave can have slaves - like a graph). It allows distributing the load across machines and making use of memory of all the machines in the cluster (also shared bandwidth)._x000a_Failover:_x000a_Redis Sentinal helps to manage Redis instances. If a master goes down, Sentinal automatically starts a process that can promote Slave node into Master._x000a_Also, it updates the clients to use new master instead of the old._x000a_Note: Redis configurations are eventually-consistent._x000a_Connections:_x000a_Redis uses multiplexing and non-blocking I/O techniques to handle incoming connections. It just increases the availability of the Redis instance._x000a_Recovery:_x000a_One of the major problem with large scale is, How to recover incase of failover. Redis Persistence can address this. The RDB persistence performs point-in-time snapshots of your dataset at specified intervals. These snapshots are completely configurable and can be transferred to different datacenter for recovery purposes." xr:uid="{25CC01B7-3574-489A-818D-70D793877ADC}"/>
+    <hyperlink ref="H13" r:id="rId1" display="https://www.quora.com/How-scalable-is-Redis                                            Partitioning:_x000a_Since the data is in key-value format, its easy to distribute them into different partitions. In this way, we don't have to rely on a single computer. Same time, the overall capacity of Redis instance is equal to the number of machines in the cluster (i.e., it can make use of complete resources in your cluster)._x000a_Replication:_x000a_Redis follows master-slave replication, that means you can have one master and many slaves (and each slave can have slaves - like a graph). It allows distributing the load across machines and making use of memory of all the machines in the cluster (also shared bandwidth)._x000a_Failover:_x000a_Redis Sentinal helps to manage Redis instances. If a master goes down, Sentinal automatically starts a process that can promote Slave node into Master._x000a_Also, it updates the clients to use new master instead of the old._x000a_Note: Redis configurations are eventually-consistent._x000a_Connections:_x000a_Redis uses multiplexing and non-blocking I/O techniques to handle incoming connections. It just increases the availability of the Redis instance._x000a_Recovery:_x000a_One of the major problem with large scale is, How to recover incase of failover. Redis Persistence can address this. The RDB persistence performs point-in-time snapshots of your dataset at specified intervals. These snapshots are completely configurable and can be transferred to different datacenter for recovery purposes." xr:uid="{25CC01B7-3574-489A-818D-70D793877ADC}"/>
+    <hyperlink ref="I18" r:id="rId2" xr:uid="{A5CD4ADF-4038-41BC-8106-D01C2C90DE07}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Created folder for Zwischenvortrag, updated spreadsheet
</commit_message>
<xml_diff>
--- a/KeyValueDatabases.xlsx
+++ b/KeyValueDatabases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anthonys_Documents\Uni_Stuttgart\Forschungsprojekt\Key-Value-Datenspeichern-FP-2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BBD2C55-8E9E-4232-9EC2-8A2B34A06A8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75FD6E71-B347-4E4B-A22E-4FFA6E1551BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1245" yWindow="8190" windowWidth="37155" windowHeight="12810" activeTab="1" xr2:uid="{92F50C3F-08B8-4F3D-A3AD-7E997F6070BE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{92F50C3F-08B8-4F3D-A3AD-7E997F6070BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="175">
   <si>
     <t>Vergleich von Key-Value Datenspeichern</t>
   </si>
@@ -626,6 +626,12 @@
   <si>
     <t>https://github.com/h2database/h2database/blob/master/h2/src/docsrc/html/mvstore.html
 315-317</t>
+  </si>
+  <si>
+    <t>mit installer/von zip Datei unzippen</t>
+  </si>
+  <si>
+    <t>es existieren Clients (z.B Java (letzter Commit: 09.06.2021)), odermit Docker selbst eine image bauen/file pullen</t>
   </si>
 </sst>
 </file>
@@ -1822,10 +1828,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BFE27C2-1312-4A04-AF7F-1C5ECB1703A1}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17:I18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1838,9 +1844,10 @@
     <col min="6" max="6" width="27.42578125" customWidth="1"/>
     <col min="7" max="7" width="36.42578125" customWidth="1"/>
     <col min="8" max="8" width="27.42578125" customWidth="1"/>
+    <col min="9" max="9" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1866,64 +1873,67 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>103</v>
+        <v>78</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="157.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="157.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>11</v>
+        <v>166</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>104</v>
+        <v>167</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>78</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>105</v>
+        <v>173</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>106</v>
+        <v>170</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="141" customHeight="1" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="141" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>118</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>69</v>
+        <v>31</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>17</v>
@@ -1932,363 +1942,104 @@
         <v>18</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>130</v>
+        <v>23</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>78</v>
+        <v>112</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>79</v>
+        <v>113</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>113</v>
+        <v>174</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="204" customHeight="1" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="204" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="141" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="229.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-    </row>
-    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-    </row>
-    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-    </row>
-    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="195" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="I18" s="7" t="s">
-        <v>172</v>
-      </c>
-    </row>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:9" ht="82.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:9" ht="141" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:9" ht="113.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:9" ht="229.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H13" r:id="rId1" display="https://www.quora.com/How-scalable-is-Redis                                            Partitioning:_x000a_Since the data is in key-value format, its easy to distribute them into different partitions. In this way, we don't have to rely on a single computer. Same time, the overall capacity of Redis instance is equal to the number of machines in the cluster (i.e., it can make use of complete resources in your cluster)._x000a_Replication:_x000a_Redis follows master-slave replication, that means you can have one master and many slaves (and each slave can have slaves - like a graph). It allows distributing the load across machines and making use of memory of all the machines in the cluster (also shared bandwidth)._x000a_Failover:_x000a_Redis Sentinal helps to manage Redis instances. If a master goes down, Sentinal automatically starts a process that can promote Slave node into Master._x000a_Also, it updates the clients to use new master instead of the old._x000a_Note: Redis configurations are eventually-consistent._x000a_Connections:_x000a_Redis uses multiplexing and non-blocking I/O techniques to handle incoming connections. It just increases the availability of the Redis instance._x000a_Recovery:_x000a_One of the major problem with large scale is, How to recover incase of failover. Redis Persistence can address this. The RDB persistence performs point-in-time snapshots of your dataset at specified intervals. These snapshots are completely configurable and can be transferred to different datacenter for recovery purposes." xr:uid="{25CC01B7-3574-489A-818D-70D793877ADC}"/>
-    <hyperlink ref="I18" r:id="rId2" xr:uid="{A5CD4ADF-4038-41BC-8106-D01C2C90DE07}"/>
+    <hyperlink ref="I3" r:id="rId1" xr:uid="{A5CD4ADF-4038-41BC-8106-D01C2C90DE07}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>